<commit_message>
profile image and projects
</commit_message>
<xml_diff>
--- a/upload/template/role/Bulk Upload Template.xlsx
+++ b/upload/template/role/Bulk Upload Template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
   <si>
     <t xml:space="preserve">Sr. No</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t xml:space="preserve">E0124</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pratiksha Sanam</t>
   </si>
   <si>
     <t xml:space="preserve">.NET Developer</t>
@@ -380,7 +377,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="B3 B9"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -465,7 +462,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -612,16 +609,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>30</v>
-      </c>
+      <c r="C5" s="6"/>
       <c r="D5" s="7" t="n">
         <v>44921</v>
       </c>
@@ -629,10 +624,10 @@
         <v>35952</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>20</v>
@@ -649,10 +644,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="D6" s="7" t="n">
         <v>44922</v>
@@ -664,7 +659,7 @@
         <v>18</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>20</v>
@@ -681,10 +676,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="D7" s="7" t="n">
         <v>44923</v>
@@ -693,13 +688,13 @@
         <v>35952</v>
       </c>
       <c r="F7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="H7" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="I7" s="9" t="n">
         <v>9823546721</v>
@@ -713,10 +708,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="D8" s="7" t="n">
         <v>44924</v>
@@ -728,10 +723,10 @@
         <v>24</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I8" s="9" t="n">
         <v>9052086452</v>
@@ -745,10 +740,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="7" t="n">
         <v>44925</v>
@@ -757,13 +752,13 @@
         <v>35952</v>
       </c>
       <c r="F9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>46</v>
-      </c>
       <c r="H9" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I9" s="9" t="n">
         <v>1209782345</v>
@@ -777,10 +772,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>48</v>
       </c>
       <c r="D10" s="7" t="n">
         <v>44926</v>
@@ -789,10 +784,10 @@
         <v>35953</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>20</v>
@@ -841,7 +836,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="1" sqref="B3 H14"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -853,10 +848,10 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -864,7 +859,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -878,7 +873,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -886,7 +881,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -900,7 +895,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
resolve bulk upload issue and add app role functionality
</commit_message>
<xml_diff>
--- a/upload/template/role/Bulk Upload Template.xlsx
+++ b/upload/template/role/Bulk Upload Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Technologies" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t xml:space="preserve">Sr. No</t>
   </si>
@@ -72,16 +72,16 @@
     <t xml:space="preserve">Location</t>
   </si>
   <si>
-    <t xml:space="preserve">E0121</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pratiksha Wakekar</t>
+    <t xml:space="preserve">E0101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p1</t>
   </si>
   <si>
     <t xml:space="preserve">Solution Developer</t>
   </si>
   <si>
-    <t xml:space="preserve">pratiksha@quadwave.com</t>
+    <t xml:space="preserve">p1@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Female</t>
@@ -90,85 +90,28 @@
     <t xml:space="preserve">Pune</t>
   </si>
   <si>
-    <t xml:space="preserve">E0123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mrunali Desai</t>
+    <t xml:space="preserve">E0102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p2</t>
   </si>
   <si>
     <t xml:space="preserve">Java Developer</t>
   </si>
   <si>
-    <t xml:space="preserve">mrunali@quadwave.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suraksha Nigade</t>
+    <t xml:space="preserve">p2@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E0103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p3</t>
   </si>
   <si>
     <t xml:space="preserve">Test Engineer</t>
   </si>
   <si>
-    <t xml:space="preserve">suraksha@quadwave.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E0124</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.NET Developer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pratiksha.s@quadwave.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E0125</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ranjana Mishra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ranjana@quadwave.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E0126</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Devkaran</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ReactJs Developer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">devkaran@quadwave.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E0127</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manish Langhe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">manish@quadwave.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sachin Rathod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Angular Developer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sachin@quadwave.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E0129</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juhi Tipale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">juhi@quadwave.com</t>
+    <t xml:space="preserve">p3@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Sr.No</t>
@@ -461,8 +404,8 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -513,7 +456,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
@@ -545,7 +488,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
@@ -559,7 +502,7 @@
         <v>44919</v>
       </c>
       <c r="E3" s="7" t="n">
-        <v>36657</v>
+        <v>35953</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>24</v>
@@ -577,15 +520,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" s="7" t="n">
         <v>44920</v>
@@ -594,10 +537,10 @@
         <v>35952</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>20</v>
@@ -609,211 +552,19 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7" t="n">
-        <v>44921</v>
-      </c>
-      <c r="E5" s="7" t="n">
-        <v>35952</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="9" t="n">
-        <v>9856432111</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="7" t="n">
-        <v>44922</v>
-      </c>
-      <c r="E6" s="7" t="n">
-        <v>37291</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="9" t="n">
-        <v>9823457281</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="7" t="n">
-        <v>44923</v>
-      </c>
-      <c r="E7" s="7" t="n">
-        <v>35952</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="9" t="n">
-        <v>9823546721</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="7" t="n">
-        <v>44924</v>
-      </c>
-      <c r="E8" s="7" t="n">
-        <v>35952</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="9" t="n">
-        <v>9052086452</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="7" t="n">
-        <v>44925</v>
-      </c>
-      <c r="E9" s="7" t="n">
-        <v>35952</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="9" t="n">
-        <v>1209782345</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="7" t="n">
-        <v>44926</v>
-      </c>
-      <c r="E10" s="7" t="n">
-        <v>35953</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>4123487659</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="pratiksha@quadwave.com"/>
-    <hyperlink ref="G3" r:id="rId2" display="mrunali@quadwave.com"/>
-    <hyperlink ref="G4" r:id="rId3" display="suraksha@quadwave.com"/>
-    <hyperlink ref="G5" r:id="rId4" display="pratiksha.s@quadwave.com"/>
-    <hyperlink ref="G6" r:id="rId5" display="ranjana@quadwave.com"/>
-    <hyperlink ref="G7" r:id="rId6" display="devkaran@quadwave.com"/>
-    <hyperlink ref="G8" r:id="rId7" display="manish@quadwave.com"/>
-    <hyperlink ref="G9" r:id="rId8" display="sachin@quadwave.com"/>
-    <hyperlink ref="G10" r:id="rId9" display="juhi@quadwave.com"/>
+    <hyperlink ref="G2" r:id="rId1" display="p1@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -823,7 +574,7 @@
     <oddFooter/>
   </headerFooter>
   <tableParts>
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -833,10 +584,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -848,10 +599,10 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -859,21 +610,23 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="10" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -881,21 +634,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>53</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resolve edit employee issue
</commit_message>
<xml_diff>
--- a/upload/template/role/Bulk Upload Template.xlsx
+++ b/upload/template/role/Bulk Upload Template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
   <si>
     <t xml:space="preserve">Sr. No</t>
   </si>
@@ -130,6 +130,60 @@
   </si>
   <si>
     <t xml:space="preserve">p14@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E0115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p15@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E0119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p19@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E0120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p20@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E0121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p21@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E0122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p22@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E0123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p23@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Sr.No</t>
@@ -428,10 +482,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -607,7 +661,7 @@
         <v>35953</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>32</v>
@@ -658,6 +712,208 @@
       </c>
       <c r="K6" s="3" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="9" t="n">
+        <v>44922</v>
+      </c>
+      <c r="E7" s="9" t="n">
+        <v>35954</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="11" t="n">
+        <v>1234543268</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="9" t="n">
+        <v>44922</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>35967</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="11" t="n">
+        <v>1234543268</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>44922</v>
+      </c>
+      <c r="E9" s="9" t="n">
+        <v>35959</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="11" t="n">
+        <v>1234543268</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="9" t="n">
+        <v>44922</v>
+      </c>
+      <c r="E10" s="9" t="n">
+        <v>35964</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="11" t="n">
+        <v>1234543268</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="9" t="n">
+        <v>44922</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <v>35964</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="9" t="n">
+        <v>44922</v>
+      </c>
+      <c r="E12" s="9" t="n">
+        <v>35964</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="3" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -697,10 +953,10 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -708,7 +964,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -724,7 +980,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,7 +988,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -748,7 +1004,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Store the user profile in project path (EmployeeId is a folder name)
</commit_message>
<xml_diff>
--- a/upload/template/role/Bulk Upload Template.xlsx
+++ b/upload/template/role/Bulk Upload Template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
   <si>
     <t xml:space="preserve">Sr. No</t>
   </si>
@@ -184,6 +184,15 @@
   </si>
   <si>
     <t xml:space="preserve">p23@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E0124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p24@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Sr.No</t>
@@ -482,10 +491,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -903,7 +912,9 @@
       <c r="E12" s="9" t="n">
         <v>35964</v>
       </c>
-      <c r="F12" s="8"/>
+      <c r="F12" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="G12" s="10" t="s">
         <v>53</v>
       </c>
@@ -913,6 +924,41 @@
       <c r="I12" s="11"/>
       <c r="J12" s="8"/>
       <c r="K12" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="9" t="n">
+        <v>45287</v>
+      </c>
+      <c r="E13" s="9" t="n">
+        <v>36329</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="11" t="n">
+        <v>1234543268</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -953,10 +999,10 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -964,7 +1010,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -980,7 +1026,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -988,7 +1034,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1004,7 +1050,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>